<commit_message>
Plakat / Broschüre 1. draft
</commit_message>
<xml_diff>
--- a/Dokumentation/HardwareVorschlaege.xlsx
+++ b/Dokumentation/HardwareVorschlaege.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,20 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Bezeichnung</t>
   </si>
   <si>
-    <t>IO-Link Schnittstelle vorhanden</t>
-  </si>
-  <si>
     <t>Verfügbarkeit</t>
   </si>
   <si>
-    <t>Verkauf über</t>
-  </si>
-  <si>
     <t>Preis</t>
   </si>
   <si>
@@ -47,9 +41,6 @@
     <t>SK-16FX-EUROSCOPE -&gt; Motherboard</t>
   </si>
   <si>
-    <t>IO-Link Shield</t>
-  </si>
-  <si>
     <t>auf Anfrage</t>
   </si>
   <si>
@@ -65,9 +56,6 @@
     <t>nirgends zum Verkauf</t>
   </si>
   <si>
-    <t>nur mit Pin</t>
-  </si>
-  <si>
     <t>DC2227A - LT3669-2 Demo Board</t>
   </si>
   <si>
@@ -104,12 +92,6 @@
     <t>100 Euro</t>
   </si>
   <si>
-    <t>UART or SPI or Debugger/Programmer</t>
-  </si>
-  <si>
-    <t>GPIO or Debugger/Programmer</t>
-  </si>
-  <si>
     <t>115 Euro</t>
   </si>
   <si>
@@ -140,7 +122,13 @@
     <t>SPI</t>
   </si>
   <si>
-    <t>Genügend GPIO Pins vorhanden</t>
+    <t>Verkauf via</t>
+  </si>
+  <si>
+    <t>Genügend GPIO Pins</t>
+  </si>
+  <si>
+    <t>UART oder SPI oder Debugger/ Programmer</t>
   </si>
 </sst>
 </file>
@@ -202,11 +190,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -487,218 +484,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>